<commit_message>
Avances endpoints transacciones y stocks
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t xml:space="preserve">roles</t>
   </si>
@@ -79,58 +79,61 @@
     <t xml:space="preserve">cedula</t>
   </si>
   <si>
+    <t xml:space="preserve">tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cantidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipoCategorias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idTipoCategoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">idcategoria</t>
   </si>
   <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cantidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">observacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tipoCategorias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idTipoCategoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tipo</t>
-  </si>
-  <si>
     <t xml:space="preserve">nombre</t>
   </si>
   <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">precio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categorias</t>
+  </si>
+  <si>
     <t xml:space="preserve">stock</t>
   </si>
   <si>
-    <t xml:space="preserve">`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">precio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categorias</t>
+    <t xml:space="preserve">idStock</t>
   </si>
   <si>
     <t xml:space="preserve">categoria</t>
@@ -143,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,12 +167,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
     <font>
@@ -247,15 +244,15 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -274,7 +271,7 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin"/>
@@ -306,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -351,27 +348,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -383,7 +376,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,11 +392,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,13 +481,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:M30"/>
+  <dimension ref="C2:M30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.91015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.33"/>
@@ -635,11 +636,11 @@
         <v>18</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="9"/>
@@ -652,11 +653,11 @@
         <v>20</v>
       </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="12"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="9"/>
@@ -669,7 +670,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="4" t="s">
         <v>22</v>
       </c>
@@ -680,7 +681,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I11" s="6"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="13"/>
       <c r="K11" s="4" t="s">
         <v>8</v>
       </c>
@@ -690,46 +691,31 @@
       <c r="M11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="12"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="12"/>
-      <c r="L13" s="10" t="s">
-        <v>1</v>
-      </c>
+      <c r="J13" s="13"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
+      <c r="J14" s="13"/>
       <c r="M14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="12"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="15"/>
+      <c r="L15" s="14"/>
       <c r="M15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
@@ -741,20 +727,19 @@
         <v>28</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="16"/>
+      <c r="I16" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="15"/>
       <c r="K16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="17" t="n">
+      <c r="M16" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
@@ -765,7 +750,7 @@
       <c r="G17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="10"/>
@@ -779,19 +764,18 @@
       <c r="M17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E18" s="9"/>
       <c r="G18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>19</v>
+      <c r="H18" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>8</v>
@@ -802,11 +786,10 @@
       <c r="M18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="9"/>
@@ -823,10 +806,11 @@
       <c r="L19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="6"/>
+      <c r="M19" s="14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -835,10 +819,13 @@
       </c>
       <c r="E20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="18" t="n">
+        <v>1</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="4" t="s">
@@ -847,104 +834,123 @@
       <c r="L20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="6"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12"/>
       <c r="D21" s="19" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="I21" s="9"/>
       <c r="J21" s="6"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="9"/>
       <c r="G22" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I22" s="9"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="M22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="9"/>
-      <c r="G23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="I23" s="9"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="M23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12"/>
       <c r="D24" s="19" t="s">
         <v>1</v>
       </c>
       <c r="E24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="M24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12"/>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="M25" s="22"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="23" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="23" t="n">
-        <v>1</v>
-      </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E26" s="5"/>
+      <c r="K26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="22"/>
+      <c r="K27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="22"/>
+        <v>38</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="K28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="4" t="s">
@@ -953,7 +959,13 @@
       <c r="D29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="22"/>
+      <c r="E29" s="24"/>
+      <c r="K29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="4" t="s">
@@ -964,7 +976,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="K3:L3"/>
@@ -972,6 +984,7 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="K25:L25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Pruebas y modificaciones de servicios
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">tipoCategorias</t>
+    <t xml:space="preserve">tiposCategorias</t>
   </si>
   <si>
     <t xml:space="preserve">productos</t>
@@ -481,10 +481,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:M30"/>
+  <dimension ref="C2:R36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,6 +784,12 @@
         <v>32</v>
       </c>
       <c r="M18" s="6"/>
+      <c r="Q18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="4" t="s">
@@ -808,6 +814,15 @@
       </c>
       <c r="M19" s="14" t="n">
         <v>1</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,6 +850,15 @@
         <v>17</v>
       </c>
       <c r="M20" s="7"/>
+      <c r="P20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>-3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="19" t="n">
@@ -854,6 +878,9 @@
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="9"/>
+      <c r="R21" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="13"/>
@@ -886,6 +913,12 @@
       <c r="E24" s="9"/>
       <c r="I24" s="9"/>
       <c r="M24" s="9"/>
+      <c r="Q24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R24" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
@@ -906,6 +939,12 @@
       <c r="M25" s="23" t="s">
         <v>1</v>
       </c>
+      <c r="P25" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="4" t="s">
@@ -920,6 +959,12 @@
       </c>
       <c r="L26" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,6 +1018,40 @@
       </c>
       <c r="D30" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P31" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P32" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q34" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P35" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P36" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>